<commit_message>
base finished chapter 8 5%
</commit_message>
<xml_diff>
--- a/autocrword/models/chapter_8/chapter8database.xlsx
+++ b/autocrword/models/chapter_8/chapter8database.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C670B01-576A-47A7-89BC-DED7AE00122B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D476BCE-7A1F-4424-BE4B-0AA8C3341D96}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="465" yWindow="1245" windowWidth="28335" windowHeight="12960" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="风机基础数据" sheetId="1" r:id="rId1"/>
@@ -1193,7 +1193,7 @@
         </row>
         <row r="5">
           <cell r="A5" t="str">
-            <v>陡坡低山</v>
+            <v>丘陵</v>
           </cell>
           <cell r="E5">
             <v>0.8</v>
@@ -1473,7 +1473,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W74"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -7691,8 +7691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CEC6D52-00C5-4DB1-97AD-7F926EC519CA}">
   <dimension ref="A1:AC19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -8705,6 +8705,7 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
base finished chapter 8 70%
</commit_message>
<xml_diff>
--- a/autocrword/models/chapter_8/chapter8database.xlsx
+++ b/autocrword/models/chapter_8/chapter8database.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E5AF25-8D6A-402A-A44B-87BF711D6632}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71577583-0725-47F9-8A0D-C530751E8E2C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-345" yWindow="1275" windowWidth="25470" windowHeight="13815" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="1620" windowWidth="25470" windowHeight="13815" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="风机基础数据" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
base finished chapter 8 75%
</commit_message>
<xml_diff>
--- a/autocrword/models/chapter_8/chapter8database.xlsx
+++ b/autocrword/models/chapter_8/chapter8database.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF1E8D9-42C6-4E44-AF56-0B85C838F67D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0049DA-9FE0-4A19-A716-234FEF1A238D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2385" yWindow="7455" windowWidth="27450" windowHeight="13830" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7740" yWindow="6630" windowWidth="27450" windowHeight="13830" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="风机基础数据" sheetId="1" r:id="rId1"/>
@@ -611,169 +611,17 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>terrain_type</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gradedgravelbase_2</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>C30concretepavement_2</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>roundtubeculvert_2</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Stonemasonrydrainageditch_2</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>mortarstoneretainingwall_2</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Turfslopeprotection_2</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>Signage_2</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>Waveguardrail_2</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gradedgravelpavement_1</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>roundtubeculvert_1</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Stonemasonrydrainageditch_1</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>mortarstoneretainingwall_1</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Turfslopeprotection_1</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>桥梁</t>
-  </si>
-  <si>
-    <t>Mountainpavement_3</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>C30concretepavement_3</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>roundtubeculvert_3</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Stonemasonrydrainageditch_3</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>mortarstoneretainingwall_3</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Turfslopeprotection_3</t>
-    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Signage_3</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>Waveguardrail_3</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Landuse_3</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Earthexcavation_1</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Stoneexcavation_1</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Earthworkbackfill_1</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Earthexcavation_2</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Stoneexcavation_2</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Earthworkbackfill_2</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Earthexcavation_3</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Stoneexcavation_3</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Earthworkbackfill_3</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>bridge_3</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Generalsiteleveling_4</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Stonemasonrydrainageditch_4</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>mortarstoneprotectionslope_4</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Turfslopeprotection_4</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Earthexcavation_4</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Stoneexcavation_4</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Earthworkbackfill_4</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>FortificationIntensity</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -952,6 +800,158 @@
   <si>
     <t>LightningRod</t>
     <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>TerrainType</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>GradedGravelPavement_1</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>RoundTubeCulvert_1</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>StoneMasonryDrainageDitch_1</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>MortarStoneRetainingWall_1</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>TurfSlopeProtection_1</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>EarthExcavation_RoadBase_1</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>StoneExcavation_RoadBase_1</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>EarthWorkBackFill_RoadBase_1</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>GradedGravelBase_2</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>C30ConcretePavement_2</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>RoundTubeCulvert_2</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>StoneMasonryDrainageDitch_2</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>MortarStoneRetainingWall_2</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>WaveGuardrail_2</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>EarthExcavation_RoadBase_2</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>StoneExcavation_RoadBase_2</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>EarthWorkBackFill_RoadBase_2</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>MountainPavement_3</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>C30ConcretePavement_3</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>RoundTubeCulvert_3</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>StoneMasonryDrainageDitch_3</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>MortarStoneRetainingWall_3</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>TurfSlopeProtection_3</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>WaveGuardrail_3</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>LandUse_3</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>EarthExcavation_RoadBase_3</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>StoneExcavation_RoadBase_3</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>EarthWorkBackFill_RoadBase_3</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bridge_3</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>GeneralSiteLeveling_4</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>StoneMasonryDrainageDitch_4</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>MortarStoneProtectionSlope_4</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>TurfSlopeProtection_4</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>EarthExcavation_RoadBase_4</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>StoneExcavation_RoadBase_4</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>EarthWorkBackFill_RoadBase_4</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>TurfSlopeProtection_2</t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1717,19 +1717,19 @@
     </row>
     <row r="2" spans="1:23" s="22" customFormat="1" ht="15">
       <c r="A2" s="22" t="s">
-        <v>150</v>
+        <v>112</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>151</v>
+        <v>113</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>152</v>
+        <v>114</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>153</v>
+        <v>115</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>154</v>
+        <v>116</v>
       </c>
       <c r="F2" s="22" t="s">
         <v>96</v>
@@ -1747,16 +1747,16 @@
         <v>95</v>
       </c>
       <c r="K2" s="22" t="s">
-        <v>155</v>
+        <v>117</v>
       </c>
       <c r="L2" s="22" t="s">
-        <v>156</v>
+        <v>118</v>
       </c>
       <c r="M2" s="22" t="s">
-        <v>157</v>
+        <v>119</v>
       </c>
       <c r="N2" s="22" t="s">
-        <v>158</v>
+        <v>120</v>
       </c>
       <c r="O2" s="22" t="s">
         <v>98</v>
@@ -1768,19 +1768,19 @@
         <v>100</v>
       </c>
       <c r="R2" s="22" t="s">
-        <v>159</v>
+        <v>121</v>
       </c>
       <c r="S2" s="22" t="s">
-        <v>160</v>
+        <v>122</v>
       </c>
       <c r="U2" s="22" t="s">
-        <v>161</v>
+        <v>123</v>
       </c>
       <c r="V2" s="22" t="s">
-        <v>162</v>
+        <v>124</v>
       </c>
       <c r="W2" s="22" t="s">
-        <v>163</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:23">
@@ -7351,34 +7351,34 @@
     </row>
     <row r="3" spans="1:16" s="22" customFormat="1" ht="15">
       <c r="A3" s="22" t="s">
-        <v>164</v>
+        <v>126</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>165</v>
+        <v>127</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>166</v>
+        <v>128</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>167</v>
+        <v>129</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>168</v>
+        <v>130</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>169</v>
+        <v>131</v>
       </c>
       <c r="G3" s="22" t="s">
-        <v>170</v>
+        <v>132</v>
       </c>
       <c r="H3" s="22" t="s">
-        <v>171</v>
+        <v>133</v>
       </c>
       <c r="I3" s="22" t="s">
-        <v>172</v>
+        <v>134</v>
       </c>
       <c r="J3" s="22" t="s">
-        <v>173</v>
+        <v>135</v>
       </c>
       <c r="K3" s="22" t="s">
         <v>105</v>
@@ -7844,17 +7844,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CEC6D52-00C5-4DB1-97AD-7F926EC519CA}">
   <dimension ref="A1:AC19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="X3" sqref="X3"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="30.375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.75" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29.375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="28.375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="30.375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="24.625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.75" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
@@ -8031,76 +8054,76 @@
     </row>
     <row r="3" spans="1:29" ht="15">
       <c r="A3" s="22" t="s">
-        <v>174</v>
+        <v>136</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>175</v>
+        <v>137</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>176</v>
+        <v>138</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>166</v>
+        <v>128</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>167</v>
+        <v>129</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>177</v>
+        <v>139</v>
       </c>
       <c r="G3" s="22" t="s">
-        <v>178</v>
+        <v>140</v>
       </c>
       <c r="H3" s="22" t="s">
-        <v>179</v>
+        <v>141</v>
       </c>
       <c r="I3" s="22" t="s">
-        <v>180</v>
+        <v>142</v>
       </c>
       <c r="J3" s="22" t="s">
-        <v>181</v>
+        <v>143</v>
       </c>
       <c r="K3" s="22" t="s">
-        <v>182</v>
+        <v>144</v>
       </c>
       <c r="L3" s="22" t="s">
-        <v>183</v>
+        <v>145</v>
       </c>
       <c r="M3" s="22" t="s">
-        <v>184</v>
+        <v>146</v>
       </c>
       <c r="N3" s="22" t="s">
-        <v>185</v>
+        <v>147</v>
       </c>
       <c r="O3" s="22" t="s">
-        <v>186</v>
+        <v>148</v>
       </c>
       <c r="P3" s="22" t="s">
-        <v>187</v>
+        <v>149</v>
       </c>
       <c r="Q3" s="22" t="s">
-        <v>188</v>
+        <v>150</v>
       </c>
       <c r="R3" s="22" t="s">
-        <v>189</v>
+        <v>151</v>
       </c>
       <c r="S3" s="22" t="s">
-        <v>190</v>
+        <v>152</v>
       </c>
       <c r="T3" s="22" t="s">
-        <v>191</v>
+        <v>153</v>
       </c>
       <c r="U3" s="22" t="s">
         <v>106</v>
       </c>
       <c r="V3" s="22" t="s">
-        <v>192</v>
+        <v>154</v>
       </c>
       <c r="W3" s="22" t="s">
-        <v>193</v>
+        <v>155</v>
       </c>
       <c r="X3" s="22" t="s">
-        <v>194</v>
+        <v>156</v>
       </c>
       <c r="Z3" s="22" t="s">
         <v>102</v>
@@ -8867,18 +8890,20 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -8941,32 +8966,32 @@
     </row>
     <row r="3" spans="1:11" ht="15">
       <c r="A3" s="6" t="s">
-        <v>109</v>
+        <v>157</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>118</v>
+        <v>158</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>119</v>
+        <v>159</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>120</v>
+        <v>160</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>121</v>
+        <v>161</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>122</v>
+        <v>162</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6" t="s">
-        <v>133</v>
+        <v>163</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>134</v>
+        <v>164</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>135</v>
+        <v>165</v>
       </c>
       <c r="K3" s="22"/>
     </row>
@@ -9261,20 +9286,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BDCBB96-49E7-4AF1-99A5-1885089E0E0E}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3:M3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="11.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.75" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -9355,41 +9384,41 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>116</v>
-      </c>
       <c r="I3" s="6" t="s">
-        <v>117</v>
+        <v>171</v>
       </c>
       <c r="J3" s="6"/>
       <c r="K3" s="6" t="s">
-        <v>136</v>
+        <v>172</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>137</v>
+        <v>173</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>138</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -9756,17 +9785,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B10D049-4633-42E3-9CD9-63531EF6C06B}">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.75" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.25" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="28.5">
@@ -9854,51 +9892,51 @@
         <v>67</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="6" t="s">
-        <v>109</v>
+        <v>157</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>124</v>
+        <v>175</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>125</v>
+        <v>176</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>126</v>
+        <v>177</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>127</v>
+        <v>178</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>128</v>
+        <v>179</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>129</v>
+        <v>180</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>131</v>
+        <v>181</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>132</v>
+        <v>182</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>139</v>
+        <v>183</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>140</v>
+        <v>184</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>141</v>
+        <v>185</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>142</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -10323,17 +10361,18 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="27.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="28" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -10378,28 +10417,28 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="6" t="s">
-        <v>109</v>
+        <v>157</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>143</v>
+        <v>187</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>144</v>
+        <v>188</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>145</v>
+        <v>189</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>146</v>
+        <v>190</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>147</v>
+        <v>191</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>148</v>
+        <v>192</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>149</v>
+        <v>193</v>
       </c>
       <c r="J3" s="18"/>
     </row>

</xml_diff>